<commit_message>
Added infinity compatible volume conversion function
</commit_message>
<xml_diff>
--- a/web/helpers/Volume Scaling Values.xlsx
+++ b/web/helpers/Volume Scaling Values.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasweber/git/TTEclipseWS/PySwitch/web/helpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B4F2BD-4B0A-5E48-9F61-CA387916105B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD304DF-B10D-1B43-A663-B5EC9C9B6503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20120" xr2:uid="{D74DAF5C-8AB4-8543-9FDF-13C33CB3A8F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -136,8 +136,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4308280230252385E-2"/>
-          <c:y val="4.7743703089745362E-2"/>
+          <c:x val="5.0580043348239997E-2"/>
+          <c:y val="4.5069897679902313E-2"/>
           <c:w val="0.93999489825385518"/>
           <c:h val="0.90625730994152043"/>
         </c:manualLayout>
@@ -290,6 +290,154 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8ED5-CD4E-A5E5-9C819CAAC0F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$1:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$1:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-148.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-81.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-48.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-36.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-34.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-33.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-26.400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-20.400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-16.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-14.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-9.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-076B-3E4E-91BE-4B6B7325FC27}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1040,16 +1188,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1394,139 +1542,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF968066-7261-3E45-B8AC-0226633EED33}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
         <v>-144</v>
       </c>
+      <c r="C1">
+        <f t="shared" ref="C1:C12" si="0">C2-D1</f>
+        <v>-148.5</v>
+      </c>
+      <c r="D1">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="E1">
+        <f>B1-C1</f>
+        <v>4.5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>-81.099999999999994</v>
       </c>
+      <c r="C2">
+        <f t="shared" si="0"/>
+        <v>-81.099999999999994</v>
+      </c>
+      <c r="D2">
+        <v>32.5</v>
+      </c>
+      <c r="E2">
+        <f>B2-C2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>-51.3</v>
       </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>-48.6</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E16" si="1">B3-C3</f>
+        <v>-2.6999999999999957</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>-36.5</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>-36.6</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0.10000000000000142</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>-35</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-34.6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>-0.39999999999999858</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>-33.5</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-33.6</v>
+      </c>
+      <c r="D6">
+        <v>7.2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.10000000000000142</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10</v>
       </c>
       <c r="B7">
         <v>-26.4</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-26.400000000000002</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20</v>
       </c>
       <c r="B8">
         <v>-20.7</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-20.400000000000002</v>
+      </c>
+      <c r="D8">
+        <v>3.6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>-0.29999999999999716</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>30</v>
       </c>
       <c r="B9">
         <v>-16.8</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-16.8</v>
+      </c>
+      <c r="D9">
+        <v>2.4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>40</v>
       </c>
       <c r="B10">
         <v>-14.4</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-14.4</v>
+      </c>
+      <c r="D10">
+        <v>2.4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>50</v>
       </c>
       <c r="B11">
         <v>-12</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="D11">
+        <v>2.4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>60</v>
       </c>
       <c r="B12">
         <v>-9.5</v>
       </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-9.6</v>
+      </c>
+      <c r="D12">
+        <v>2.4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>70</v>
       </c>
       <c r="B13">
         <v>-7.3</v>
       </c>
+      <c r="C13">
+        <f>C14-D13</f>
+        <v>-7.1999999999999993</v>
+      </c>
+      <c r="D13">
+        <v>2.4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>-0.10000000000000053</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>80</v>
       </c>
       <c r="B14">
         <v>-4.7</v>
       </c>
+      <c r="C14">
+        <f>C15-D14</f>
+        <v>-4.8</v>
+      </c>
+      <c r="D14">
+        <v>2.4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>90</v>
       </c>
       <c r="B15">
         <v>-2.4</v>
       </c>
+      <c r="C15">
+        <f>C16-D15</f>
+        <v>-2.4</v>
+      </c>
+      <c r="D15">
+        <v>2.4</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>100</v>
       </c>
       <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>